<commit_message>
UPDATE20210604 (REMOVE SHIFT, ADD SETTING & UPDATE OTOMATIS ADD OUTSTANDING TO THP QTY)
</commit_message>
<xml_diff>
--- a/public/import/test.xlsx
+++ b/public/import/test.xlsx
@@ -1482,19 +1482,19 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="38" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -2770,24 +2770,26 @@
         <v>4.333333333333333</v>
       </c>
       <c r="O9" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="P9" s="34"/>
+        <v>1000.0</v>
+      </c>
+      <c r="P9" s="34">
+        <v>1000.0</v>
+      </c>
       <c r="Q9" s="35">
-        <v>10.0</v>
-      </c>
-      <c r="R9" s="36">
-        <v>10.0</v>
-      </c>
-      <c r="S9" s="37">
+        <v>500.0</v>
+      </c>
+      <c r="R9" s="34">
+        <v>510.0</v>
+      </c>
+      <c r="S9" s="36">
         <f t="shared" ref="S9:S124" si="1">(Q9+R9)/G9</f>
-        <v>0.01282051282</v>
-      </c>
-      <c r="T9" s="38">
+        <v>0.6474358974</v>
+      </c>
+      <c r="T9" s="37">
         <f t="shared" ref="T9:T124" si="2">(Q9+R9)*H9/3600</f>
-        <v>0.05555555556</v>
-      </c>
-      <c r="U9" s="34"/>
+        <v>2.805555556</v>
+      </c>
+      <c r="U9" s="38"/>
       <c r="V9" s="39"/>
       <c r="W9" s="39"/>
       <c r="X9" s="39"/>
@@ -2826,19 +2828,23 @@
       <c r="N10" s="31">
         <v>4.333333333333333</v>
       </c>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
+      <c r="O10" s="34">
+        <v>2000.0</v>
+      </c>
+      <c r="P10" s="34">
+        <v>2000.0</v>
+      </c>
       <c r="Q10" s="30"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="37">
+      <c r="R10" s="38"/>
+      <c r="S10" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T10" s="38">
+      <c r="T10" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U10" s="34"/>
+      <c r="U10" s="38"/>
       <c r="V10" s="40"/>
       <c r="W10" s="40"/>
       <c r="X10" s="40"/>
@@ -2877,19 +2883,23 @@
       <c r="N11" s="31">
         <v>4.333333333333333</v>
       </c>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
+      <c r="O11" s="34">
+        <v>1500.0</v>
+      </c>
+      <c r="P11" s="34">
+        <v>1500.0</v>
+      </c>
       <c r="Q11" s="30"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="37">
+      <c r="R11" s="38"/>
+      <c r="S11" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T11" s="38">
+      <c r="T11" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U11" s="34"/>
+      <c r="U11" s="38"/>
       <c r="V11" s="40"/>
       <c r="W11" s="40"/>
       <c r="X11" s="40"/>
@@ -2928,19 +2938,23 @@
       <c r="N12" s="31">
         <v>4.333333333333333</v>
       </c>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
+      <c r="O12" s="34">
+        <v>2500.0</v>
+      </c>
+      <c r="P12" s="34">
+        <v>2500.0</v>
+      </c>
       <c r="Q12" s="30"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="37">
+      <c r="R12" s="38"/>
+      <c r="S12" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T12" s="38">
+      <c r="T12" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U12" s="34"/>
+      <c r="U12" s="38"/>
       <c r="V12" s="40"/>
       <c r="W12" s="40"/>
       <c r="X12" s="40"/>
@@ -2987,21 +3001,21 @@
       <c r="N13" s="31">
         <v>7.142857142857142</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="38">
         <v>1.0</v>
       </c>
-      <c r="P13" s="34"/>
+      <c r="P13" s="38"/>
       <c r="Q13" s="30"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="37">
+      <c r="R13" s="38"/>
+      <c r="S13" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T13" s="38">
+      <c r="T13" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U13" s="34"/>
+      <c r="U13" s="38"/>
       <c r="V13" s="41"/>
       <c r="W13" s="41"/>
       <c r="X13" s="41"/>
@@ -3038,19 +3052,19 @@
       <c r="N14" s="31">
         <v>2.053388090349076</v>
       </c>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="30"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="37">
+      <c r="R14" s="38"/>
+      <c r="S14" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T14" s="38">
+      <c r="T14" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U14" s="34"/>
+      <c r="U14" s="38"/>
       <c r="V14" s="41"/>
       <c r="W14" s="41"/>
       <c r="X14" s="41"/>
@@ -3087,19 +3101,19 @@
       <c r="N15" s="31">
         <v>2.688172043010753</v>
       </c>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
       <c r="Q15" s="30"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="37">
+      <c r="R15" s="38"/>
+      <c r="S15" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T15" s="38">
+      <c r="T15" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U15" s="34"/>
+      <c r="U15" s="38"/>
       <c r="V15" s="41"/>
       <c r="W15" s="41"/>
       <c r="X15" s="41"/>
@@ -3136,19 +3150,19 @@
       <c r="N16" s="31">
         <v>2.070393374741201</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
       <c r="Q16" s="30"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="37">
+      <c r="R16" s="38"/>
+      <c r="S16" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T16" s="38">
+      <c r="T16" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U16" s="34"/>
+      <c r="U16" s="38"/>
       <c r="V16" s="41"/>
       <c r="W16" s="41"/>
       <c r="X16" s="41"/>
@@ -3195,21 +3209,21 @@
       <c r="N17" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="38">
         <v>1.0</v>
       </c>
-      <c r="P17" s="34"/>
+      <c r="P17" s="38"/>
       <c r="Q17" s="30"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="37">
+      <c r="R17" s="38"/>
+      <c r="S17" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T17" s="38">
+      <c r="T17" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U17" s="34"/>
+      <c r="U17" s="38"/>
       <c r="V17" s="41"/>
       <c r="W17" s="41"/>
       <c r="X17" s="41"/>
@@ -3246,19 +3260,19 @@
       <c r="N18" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
       <c r="Q18" s="30"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="37">
+      <c r="R18" s="38"/>
+      <c r="S18" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T18" s="38">
+      <c r="T18" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U18" s="34"/>
+      <c r="U18" s="38"/>
       <c r="V18" s="41"/>
       <c r="W18" s="41"/>
       <c r="X18" s="41"/>
@@ -3295,19 +3309,19 @@
       <c r="N19" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
       <c r="Q19" s="30"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="37">
+      <c r="R19" s="38"/>
+      <c r="S19" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T19" s="38">
+      <c r="T19" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U19" s="34"/>
+      <c r="U19" s="38"/>
       <c r="V19" s="41"/>
       <c r="W19" s="41"/>
       <c r="X19" s="41"/>
@@ -3344,19 +3358,19 @@
       <c r="N20" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
       <c r="Q20" s="30"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="37">
+      <c r="R20" s="38"/>
+      <c r="S20" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T20" s="38">
+      <c r="T20" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U20" s="34"/>
+      <c r="U20" s="38"/>
       <c r="V20" s="41"/>
       <c r="W20" s="41"/>
       <c r="X20" s="41"/>
@@ -3393,19 +3407,19 @@
       <c r="N21" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
       <c r="Q21" s="30"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="37">
+      <c r="R21" s="38"/>
+      <c r="S21" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T21" s="38">
+      <c r="T21" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U21" s="34"/>
+      <c r="U21" s="38"/>
       <c r="V21" s="41"/>
       <c r="W21" s="41"/>
       <c r="X21" s="41"/>
@@ -3442,19 +3456,19 @@
       <c r="N22" s="31">
         <v>6.333333333333333</v>
       </c>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
       <c r="Q22" s="30"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="37">
+      <c r="R22" s="38"/>
+      <c r="S22" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T22" s="38">
+      <c r="T22" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U22" s="34"/>
+      <c r="U22" s="38"/>
       <c r="V22" s="41"/>
       <c r="W22" s="41"/>
       <c r="X22" s="41"/>
@@ -3501,21 +3515,21 @@
       <c r="N23" s="31">
         <v>5.555555555555555</v>
       </c>
-      <c r="O23" s="34">
+      <c r="O23" s="38">
         <v>1.0</v>
       </c>
-      <c r="P23" s="34"/>
+      <c r="P23" s="38"/>
       <c r="Q23" s="30"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="37">
+      <c r="R23" s="38"/>
+      <c r="S23" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T23" s="38">
+      <c r="T23" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U23" s="34"/>
+      <c r="U23" s="38"/>
       <c r="V23" s="41"/>
       <c r="W23" s="41"/>
       <c r="X23" s="41"/>
@@ -3552,19 +3566,19 @@
       <c r="N24" s="31">
         <v>4.444444444444445</v>
       </c>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
       <c r="Q24" s="30"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="37">
+      <c r="R24" s="38"/>
+      <c r="S24" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T24" s="38">
+      <c r="T24" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U24" s="34"/>
+      <c r="U24" s="38"/>
       <c r="V24" s="41"/>
       <c r="W24" s="41"/>
       <c r="X24" s="41"/>
@@ -3601,19 +3615,19 @@
       <c r="N25" s="31">
         <v>3.888888888888889</v>
       </c>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
       <c r="Q25" s="30"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="37">
+      <c r="R25" s="38"/>
+      <c r="S25" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T25" s="38">
+      <c r="T25" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U25" s="34"/>
+      <c r="U25" s="38"/>
       <c r="V25" s="41"/>
       <c r="W25" s="41"/>
       <c r="X25" s="41"/>
@@ -3650,19 +3664,19 @@
       <c r="N26" s="31">
         <v>6.111111111111111</v>
       </c>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
       <c r="Q26" s="30"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="37">
+      <c r="R26" s="38"/>
+      <c r="S26" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T26" s="38">
+      <c r="T26" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U26" s="34"/>
+      <c r="U26" s="38"/>
       <c r="V26" s="41"/>
       <c r="W26" s="41"/>
       <c r="X26" s="41"/>
@@ -3709,21 +3723,21 @@
       <c r="N27" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O27" s="34">
+      <c r="O27" s="38">
         <v>1.0</v>
       </c>
-      <c r="P27" s="34"/>
+      <c r="P27" s="38"/>
       <c r="Q27" s="30"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="37">
+      <c r="R27" s="38"/>
+      <c r="S27" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T27" s="38">
+      <c r="T27" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U27" s="34"/>
+      <c r="U27" s="38"/>
       <c r="V27" s="41"/>
       <c r="W27" s="41"/>
       <c r="X27" s="41"/>
@@ -3760,19 +3774,19 @@
       <c r="N28" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
       <c r="Q28" s="30"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="37">
+      <c r="R28" s="38"/>
+      <c r="S28" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T28" s="38">
+      <c r="T28" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U28" s="34"/>
+      <c r="U28" s="38"/>
       <c r="V28" s="41"/>
       <c r="W28" s="41"/>
       <c r="X28" s="41"/>
@@ -3809,19 +3823,19 @@
       <c r="N29" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
       <c r="Q29" s="30"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="37">
+      <c r="R29" s="38"/>
+      <c r="S29" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T29" s="38">
+      <c r="T29" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U29" s="34"/>
+      <c r="U29" s="38"/>
       <c r="V29" s="41"/>
       <c r="W29" s="41"/>
       <c r="X29" s="41"/>
@@ -3858,19 +3872,19 @@
       <c r="N30" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
       <c r="Q30" s="30"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="37">
+      <c r="R30" s="38"/>
+      <c r="S30" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T30" s="38">
+      <c r="T30" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U30" s="34"/>
+      <c r="U30" s="38"/>
       <c r="V30" s="41"/>
       <c r="W30" s="41"/>
       <c r="X30" s="41"/>
@@ -3907,19 +3921,19 @@
       <c r="N31" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O31" s="34"/>
-      <c r="P31" s="34"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
       <c r="Q31" s="30"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="37">
+      <c r="R31" s="38"/>
+      <c r="S31" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T31" s="38">
+      <c r="T31" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U31" s="34"/>
+      <c r="U31" s="38"/>
       <c r="V31" s="41"/>
       <c r="W31" s="41"/>
       <c r="X31" s="41"/>
@@ -3966,21 +3980,21 @@
       <c r="N32" s="31">
         <v>2.6666666666666665</v>
       </c>
-      <c r="O32" s="34">
+      <c r="O32" s="38">
         <v>1.0</v>
       </c>
-      <c r="P32" s="34"/>
+      <c r="P32" s="38"/>
       <c r="Q32" s="30"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="37">
+      <c r="R32" s="38"/>
+      <c r="S32" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T32" s="38">
+      <c r="T32" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U32" s="34"/>
+      <c r="U32" s="38"/>
       <c r="V32" s="41"/>
       <c r="W32" s="41"/>
       <c r="X32" s="41"/>
@@ -4017,19 +4031,19 @@
       <c r="N33" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O33" s="34"/>
-      <c r="P33" s="34"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
       <c r="Q33" s="30"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="37">
+      <c r="R33" s="38"/>
+      <c r="S33" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T33" s="38">
+      <c r="T33" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U33" s="34"/>
+      <c r="U33" s="38"/>
       <c r="V33" s="41"/>
       <c r="W33" s="41"/>
       <c r="X33" s="41"/>
@@ -4066,19 +4080,19 @@
       <c r="N34" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O34" s="34"/>
-      <c r="P34" s="34"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
       <c r="Q34" s="30"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="37">
+      <c r="R34" s="38"/>
+      <c r="S34" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T34" s="38">
+      <c r="T34" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U34" s="34"/>
+      <c r="U34" s="38"/>
       <c r="V34" s="41"/>
       <c r="W34" s="41"/>
       <c r="X34" s="41"/>
@@ -4115,19 +4129,19 @@
       <c r="N35" s="31">
         <v>2.3333333333333335</v>
       </c>
-      <c r="O35" s="34"/>
-      <c r="P35" s="34"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
       <c r="Q35" s="30"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="37">
+      <c r="R35" s="38"/>
+      <c r="S35" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T35" s="38">
+      <c r="T35" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U35" s="34"/>
+      <c r="U35" s="38"/>
       <c r="V35" s="41"/>
       <c r="W35" s="41"/>
       <c r="X35" s="41"/>
@@ -4164,19 +4178,19 @@
       <c r="N36" s="31">
         <v>2.3333333333333335</v>
       </c>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
       <c r="Q36" s="30"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="37">
+      <c r="R36" s="38"/>
+      <c r="S36" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T36" s="38">
+      <c r="T36" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U36" s="34"/>
+      <c r="U36" s="38"/>
       <c r="V36" s="41"/>
       <c r="W36" s="41"/>
       <c r="X36" s="41"/>
@@ -4223,21 +4237,21 @@
       <c r="N37" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O37" s="34">
+      <c r="O37" s="38">
         <v>1.0</v>
       </c>
-      <c r="P37" s="34"/>
+      <c r="P37" s="38"/>
       <c r="Q37" s="30"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="37">
+      <c r="R37" s="38"/>
+      <c r="S37" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T37" s="38">
+      <c r="T37" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U37" s="34"/>
+      <c r="U37" s="38"/>
       <c r="V37" s="41"/>
       <c r="W37" s="41"/>
       <c r="X37" s="41"/>
@@ -4274,19 +4288,19 @@
       <c r="N38" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
       <c r="Q38" s="30"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="37">
+      <c r="R38" s="38"/>
+      <c r="S38" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T38" s="38">
+      <c r="T38" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U38" s="34"/>
+      <c r="U38" s="38"/>
       <c r="V38" s="41"/>
       <c r="W38" s="41"/>
       <c r="X38" s="41"/>
@@ -4323,19 +4337,19 @@
       <c r="N39" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
       <c r="Q39" s="30"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="37">
+      <c r="R39" s="38"/>
+      <c r="S39" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T39" s="38">
+      <c r="T39" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U39" s="34"/>
+      <c r="U39" s="38"/>
       <c r="V39" s="41"/>
       <c r="W39" s="41"/>
       <c r="X39" s="41"/>
@@ -4372,19 +4386,19 @@
       <c r="N40" s="31">
         <v>3.111111111111111</v>
       </c>
-      <c r="O40" s="34"/>
-      <c r="P40" s="34"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
       <c r="Q40" s="30"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="37">
+      <c r="R40" s="38"/>
+      <c r="S40" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T40" s="38">
+      <c r="T40" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U40" s="34"/>
+      <c r="U40" s="38"/>
       <c r="V40" s="41"/>
       <c r="W40" s="41"/>
       <c r="X40" s="41"/>
@@ -4421,19 +4435,19 @@
       <c r="N41" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O41" s="34"/>
-      <c r="P41" s="34"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
       <c r="Q41" s="30"/>
-      <c r="R41" s="34"/>
-      <c r="S41" s="37">
+      <c r="R41" s="38"/>
+      <c r="S41" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T41" s="38">
+      <c r="T41" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U41" s="34"/>
+      <c r="U41" s="38"/>
       <c r="V41" s="41"/>
       <c r="W41" s="41"/>
       <c r="X41" s="41"/>
@@ -4470,19 +4484,19 @@
       <c r="N42" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O42" s="34"/>
-      <c r="P42" s="34"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
       <c r="Q42" s="30"/>
-      <c r="R42" s="34"/>
-      <c r="S42" s="37">
+      <c r="R42" s="38"/>
+      <c r="S42" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T42" s="38">
+      <c r="T42" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U42" s="34"/>
+      <c r="U42" s="38"/>
       <c r="V42" s="41"/>
       <c r="W42" s="41"/>
       <c r="X42" s="41"/>
@@ -4529,21 +4543,21 @@
       <c r="N43" s="31">
         <v>5.0</v>
       </c>
-      <c r="O43" s="34">
+      <c r="O43" s="38">
         <v>1.0</v>
       </c>
-      <c r="P43" s="34"/>
+      <c r="P43" s="38"/>
       <c r="Q43" s="30"/>
-      <c r="R43" s="34"/>
-      <c r="S43" s="37">
+      <c r="R43" s="38"/>
+      <c r="S43" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T43" s="38">
+      <c r="T43" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U43" s="34"/>
+      <c r="U43" s="38"/>
       <c r="V43" s="41"/>
       <c r="W43" s="41"/>
       <c r="X43" s="41"/>
@@ -4580,19 +4594,19 @@
       <c r="N44" s="31">
         <v>5.0</v>
       </c>
-      <c r="O44" s="34"/>
-      <c r="P44" s="34"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
       <c r="Q44" s="30"/>
-      <c r="R44" s="34"/>
-      <c r="S44" s="37">
+      <c r="R44" s="38"/>
+      <c r="S44" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T44" s="38">
+      <c r="T44" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U44" s="34"/>
+      <c r="U44" s="38"/>
       <c r="V44" s="41"/>
       <c r="W44" s="41"/>
       <c r="X44" s="41"/>
@@ -4629,19 +4643,19 @@
       <c r="N45" s="31">
         <v>5.0</v>
       </c>
-      <c r="O45" s="34"/>
-      <c r="P45" s="34"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="38"/>
       <c r="Q45" s="30"/>
-      <c r="R45" s="34"/>
-      <c r="S45" s="37">
+      <c r="R45" s="38"/>
+      <c r="S45" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T45" s="38">
+      <c r="T45" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U45" s="34"/>
+      <c r="U45" s="38"/>
       <c r="V45" s="41"/>
       <c r="W45" s="41"/>
       <c r="X45" s="41"/>
@@ -4688,21 +4702,21 @@
       <c r="N46" s="31">
         <v>2.7777777777777777</v>
       </c>
-      <c r="O46" s="34">
+      <c r="O46" s="38">
         <v>1.0</v>
       </c>
-      <c r="P46" s="34"/>
+      <c r="P46" s="38"/>
       <c r="Q46" s="30"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="37">
+      <c r="R46" s="38"/>
+      <c r="S46" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T46" s="38">
+      <c r="T46" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U46" s="34"/>
+      <c r="U46" s="38"/>
       <c r="V46" s="41"/>
       <c r="W46" s="41"/>
       <c r="X46" s="41"/>
@@ -4739,19 +4753,19 @@
       <c r="N47" s="31">
         <v>2.7777777777777777</v>
       </c>
-      <c r="O47" s="34"/>
-      <c r="P47" s="34"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
       <c r="Q47" s="30"/>
-      <c r="R47" s="34"/>
-      <c r="S47" s="37">
+      <c r="R47" s="38"/>
+      <c r="S47" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T47" s="38">
+      <c r="T47" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U47" s="34"/>
+      <c r="U47" s="38"/>
       <c r="V47" s="41"/>
       <c r="W47" s="41"/>
       <c r="X47" s="41"/>
@@ -4798,21 +4812,21 @@
       <c r="N48" s="31">
         <v>3.1166666666666667</v>
       </c>
-      <c r="O48" s="34">
+      <c r="O48" s="38">
         <v>1.0</v>
       </c>
-      <c r="P48" s="34"/>
+      <c r="P48" s="38"/>
       <c r="Q48" s="30"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="37">
+      <c r="R48" s="38"/>
+      <c r="S48" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T48" s="38">
+      <c r="T48" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U48" s="34"/>
+      <c r="U48" s="38"/>
       <c r="V48" s="41"/>
       <c r="W48" s="41"/>
       <c r="X48" s="41"/>
@@ -4859,21 +4873,21 @@
       <c r="N49" s="31">
         <v>3.1166666666666667</v>
       </c>
-      <c r="O49" s="34">
+      <c r="O49" s="38">
         <v>1.0</v>
       </c>
-      <c r="P49" s="34"/>
+      <c r="P49" s="38"/>
       <c r="Q49" s="30"/>
-      <c r="R49" s="34"/>
-      <c r="S49" s="37">
+      <c r="R49" s="38"/>
+      <c r="S49" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T49" s="38">
+      <c r="T49" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U49" s="34"/>
+      <c r="U49" s="38"/>
       <c r="V49" s="41"/>
       <c r="W49" s="41"/>
       <c r="X49" s="41"/>
@@ -4910,19 +4924,19 @@
       <c r="N50" s="31">
         <v>3.51</v>
       </c>
-      <c r="O50" s="34"/>
-      <c r="P50" s="34"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
       <c r="Q50" s="30"/>
-      <c r="R50" s="34"/>
-      <c r="S50" s="37">
+      <c r="R50" s="38"/>
+      <c r="S50" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T50" s="38">
+      <c r="T50" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U50" s="34"/>
+      <c r="U50" s="38"/>
       <c r="V50" s="41"/>
       <c r="W50" s="41"/>
       <c r="X50" s="41"/>
@@ -4969,21 +4983,21 @@
       <c r="N51" s="31">
         <v>1.3436893203883495</v>
       </c>
-      <c r="O51" s="34">
+      <c r="O51" s="38">
         <v>1.0</v>
       </c>
-      <c r="P51" s="34"/>
+      <c r="P51" s="38"/>
       <c r="Q51" s="30"/>
-      <c r="R51" s="34"/>
-      <c r="S51" s="37">
+      <c r="R51" s="38"/>
+      <c r="S51" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T51" s="38">
+      <c r="T51" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U51" s="34"/>
+      <c r="U51" s="38"/>
       <c r="V51" s="41"/>
       <c r="W51" s="41"/>
       <c r="X51" s="41"/>
@@ -5030,21 +5044,21 @@
       <c r="N52" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O52" s="34">
+      <c r="O52" s="38">
         <v>1.0</v>
       </c>
-      <c r="P52" s="34"/>
+      <c r="P52" s="38"/>
       <c r="Q52" s="30"/>
-      <c r="R52" s="34"/>
-      <c r="S52" s="37">
+      <c r="R52" s="38"/>
+      <c r="S52" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T52" s="38">
+      <c r="T52" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U52" s="34"/>
+      <c r="U52" s="38"/>
       <c r="V52" s="41"/>
       <c r="W52" s="41"/>
       <c r="X52" s="41"/>
@@ -5081,19 +5095,19 @@
       <c r="N53" s="31">
         <v>5.555555555555555</v>
       </c>
-      <c r="O53" s="34"/>
-      <c r="P53" s="34"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="38"/>
       <c r="Q53" s="30"/>
-      <c r="R53" s="34"/>
-      <c r="S53" s="37">
+      <c r="R53" s="38"/>
+      <c r="S53" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T53" s="38">
+      <c r="T53" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U53" s="34"/>
+      <c r="U53" s="38"/>
       <c r="V53" s="41"/>
       <c r="W53" s="41"/>
       <c r="X53" s="41"/>
@@ -5140,21 +5154,21 @@
       <c r="N54" s="31">
         <v>4.622222222222222</v>
       </c>
-      <c r="O54" s="34">
+      <c r="O54" s="38">
         <v>1.0</v>
       </c>
-      <c r="P54" s="34"/>
+      <c r="P54" s="38"/>
       <c r="Q54" s="30"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="37">
+      <c r="R54" s="38"/>
+      <c r="S54" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T54" s="38">
+      <c r="T54" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U54" s="34" t="s">
+      <c r="U54" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V54" s="41"/>
@@ -5191,19 +5205,19 @@
       <c r="N55" s="31">
         <v>5.138888888888889</v>
       </c>
-      <c r="O55" s="34"/>
-      <c r="P55" s="34"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
       <c r="Q55" s="30"/>
-      <c r="R55" s="34"/>
-      <c r="S55" s="37">
+      <c r="R55" s="38"/>
+      <c r="S55" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T55" s="38">
+      <c r="T55" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U55" s="34"/>
+      <c r="U55" s="38"/>
       <c r="V55" s="41"/>
       <c r="W55" s="41"/>
       <c r="X55" s="41"/>
@@ -5238,19 +5252,19 @@
       <c r="N56" s="31">
         <v>5.138888888888889</v>
       </c>
-      <c r="O56" s="34"/>
-      <c r="P56" s="34"/>
+      <c r="O56" s="38"/>
+      <c r="P56" s="38"/>
       <c r="Q56" s="30"/>
-      <c r="R56" s="34"/>
-      <c r="S56" s="37">
+      <c r="R56" s="38"/>
+      <c r="S56" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T56" s="38">
+      <c r="T56" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U56" s="34"/>
+      <c r="U56" s="38"/>
       <c r="V56" s="41"/>
       <c r="W56" s="41"/>
       <c r="X56" s="41"/>
@@ -5297,21 +5311,21 @@
       <c r="N57" s="31">
         <v>1.953125</v>
       </c>
-      <c r="O57" s="34">
+      <c r="O57" s="38">
         <v>1.0</v>
       </c>
-      <c r="P57" s="34"/>
+      <c r="P57" s="38"/>
       <c r="Q57" s="30"/>
-      <c r="R57" s="34"/>
-      <c r="S57" s="37">
+      <c r="R57" s="38"/>
+      <c r="S57" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T57" s="38">
+      <c r="T57" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U57" s="34" t="s">
+      <c r="U57" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V57" s="41"/>
@@ -5350,19 +5364,19 @@
       <c r="N58" s="31">
         <v>2.100840336134454</v>
       </c>
-      <c r="O58" s="34"/>
-      <c r="P58" s="34"/>
+      <c r="O58" s="38"/>
+      <c r="P58" s="38"/>
       <c r="Q58" s="30"/>
-      <c r="R58" s="34"/>
-      <c r="S58" s="37">
+      <c r="R58" s="38"/>
+      <c r="S58" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T58" s="38">
+      <c r="T58" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U58" s="34"/>
+      <c r="U58" s="38"/>
       <c r="V58" s="41"/>
       <c r="W58" s="41"/>
       <c r="X58" s="41"/>
@@ -5399,19 +5413,19 @@
       <c r="N59" s="31">
         <v>2.100840336134454</v>
       </c>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
+      <c r="O59" s="38"/>
+      <c r="P59" s="38"/>
       <c r="Q59" s="30"/>
-      <c r="R59" s="34"/>
-      <c r="S59" s="37">
+      <c r="R59" s="38"/>
+      <c r="S59" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T59" s="38">
+      <c r="T59" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U59" s="34"/>
+      <c r="U59" s="38"/>
       <c r="V59" s="41"/>
       <c r="W59" s="41"/>
       <c r="X59" s="41"/>
@@ -5448,19 +5462,19 @@
       <c r="N60" s="31">
         <v>2.5316455696202533</v>
       </c>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="38"/>
       <c r="Q60" s="30"/>
-      <c r="R60" s="34"/>
-      <c r="S60" s="37">
+      <c r="R60" s="38"/>
+      <c r="S60" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T60" s="38">
+      <c r="T60" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U60" s="34"/>
+      <c r="U60" s="38"/>
       <c r="V60" s="41"/>
       <c r="W60" s="41"/>
       <c r="X60" s="41"/>
@@ -5497,19 +5511,19 @@
       <c r="N61" s="31">
         <v>2.2675736961451247</v>
       </c>
-      <c r="O61" s="34"/>
-      <c r="P61" s="34"/>
+      <c r="O61" s="38"/>
+      <c r="P61" s="38"/>
       <c r="Q61" s="30"/>
-      <c r="R61" s="34"/>
-      <c r="S61" s="37">
+      <c r="R61" s="38"/>
+      <c r="S61" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T61" s="38">
+      <c r="T61" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U61" s="34"/>
+      <c r="U61" s="38"/>
       <c r="V61" s="41"/>
       <c r="W61" s="41"/>
       <c r="X61" s="41"/>
@@ -5546,19 +5560,19 @@
       <c r="N62" s="31">
         <v>2.5694444444444446</v>
       </c>
-      <c r="O62" s="34"/>
-      <c r="P62" s="34"/>
+      <c r="O62" s="38"/>
+      <c r="P62" s="38"/>
       <c r="Q62" s="30"/>
-      <c r="R62" s="34"/>
-      <c r="S62" s="37">
+      <c r="R62" s="38"/>
+      <c r="S62" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T62" s="38">
+      <c r="T62" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U62" s="34"/>
+      <c r="U62" s="38"/>
       <c r="V62" s="41"/>
       <c r="W62" s="41"/>
       <c r="X62" s="41"/>
@@ -5605,21 +5619,21 @@
       <c r="N63" s="31">
         <v>1.953125</v>
       </c>
-      <c r="O63" s="34">
+      <c r="O63" s="38">
         <v>1.0</v>
       </c>
-      <c r="P63" s="34"/>
+      <c r="P63" s="38"/>
       <c r="Q63" s="30"/>
-      <c r="R63" s="34"/>
-      <c r="S63" s="37">
+      <c r="R63" s="38"/>
+      <c r="S63" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T63" s="38">
+      <c r="T63" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U63" s="34" t="s">
+      <c r="U63" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V63" s="41"/>
@@ -5658,19 +5672,19 @@
       <c r="N64" s="31">
         <v>2.100840336134454</v>
       </c>
-      <c r="O64" s="34"/>
-      <c r="P64" s="34"/>
+      <c r="O64" s="38"/>
+      <c r="P64" s="38"/>
       <c r="Q64" s="30"/>
-      <c r="R64" s="34"/>
-      <c r="S64" s="37">
+      <c r="R64" s="38"/>
+      <c r="S64" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T64" s="38">
+      <c r="T64" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U64" s="34"/>
+      <c r="U64" s="38"/>
       <c r="V64" s="41"/>
       <c r="W64" s="41"/>
       <c r="X64" s="41"/>
@@ -5707,19 +5721,19 @@
       <c r="N65" s="31">
         <v>2.100840336134454</v>
       </c>
-      <c r="O65" s="34"/>
-      <c r="P65" s="34"/>
+      <c r="O65" s="38"/>
+      <c r="P65" s="38"/>
       <c r="Q65" s="30"/>
-      <c r="R65" s="34"/>
-      <c r="S65" s="37">
+      <c r="R65" s="38"/>
+      <c r="S65" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T65" s="38">
+      <c r="T65" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U65" s="34"/>
+      <c r="U65" s="38"/>
       <c r="V65" s="41"/>
       <c r="W65" s="41"/>
       <c r="X65" s="41"/>
@@ -5756,19 +5770,19 @@
       <c r="N66" s="31">
         <v>2.5316455696202533</v>
       </c>
-      <c r="O66" s="34"/>
-      <c r="P66" s="34"/>
+      <c r="O66" s="38"/>
+      <c r="P66" s="38"/>
       <c r="Q66" s="30"/>
-      <c r="R66" s="34"/>
-      <c r="S66" s="37">
+      <c r="R66" s="38"/>
+      <c r="S66" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T66" s="38">
+      <c r="T66" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U66" s="34"/>
+      <c r="U66" s="38"/>
       <c r="V66" s="41"/>
       <c r="W66" s="41"/>
       <c r="X66" s="41"/>
@@ -5805,19 +5819,19 @@
       <c r="N67" s="31">
         <v>2.2675736961451247</v>
       </c>
-      <c r="O67" s="34"/>
-      <c r="P67" s="34"/>
+      <c r="O67" s="38"/>
+      <c r="P67" s="38"/>
       <c r="Q67" s="30"/>
-      <c r="R67" s="34"/>
-      <c r="S67" s="37">
+      <c r="R67" s="38"/>
+      <c r="S67" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T67" s="38">
+      <c r="T67" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U67" s="34"/>
+      <c r="U67" s="38"/>
       <c r="V67" s="41"/>
       <c r="W67" s="41"/>
       <c r="X67" s="41"/>
@@ -5864,21 +5878,21 @@
       <c r="N68" s="31">
         <v>7.222222222222222</v>
       </c>
-      <c r="O68" s="34">
+      <c r="O68" s="38">
         <v>1.0</v>
       </c>
-      <c r="P68" s="34"/>
+      <c r="P68" s="38"/>
       <c r="Q68" s="30"/>
-      <c r="R68" s="34"/>
-      <c r="S68" s="37">
+      <c r="R68" s="38"/>
+      <c r="S68" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T68" s="38">
+      <c r="T68" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U68" s="34" t="s">
+      <c r="U68" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V68" s="41"/>
@@ -5915,19 +5929,19 @@
       <c r="N69" s="31">
         <v>8.333333333333334</v>
       </c>
-      <c r="O69" s="34"/>
-      <c r="P69" s="34"/>
+      <c r="O69" s="38"/>
+      <c r="P69" s="38"/>
       <c r="Q69" s="30"/>
-      <c r="R69" s="34"/>
-      <c r="S69" s="37">
+      <c r="R69" s="38"/>
+      <c r="S69" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T69" s="38">
+      <c r="T69" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U69" s="34"/>
+      <c r="U69" s="38"/>
       <c r="V69" s="41"/>
       <c r="W69" s="41"/>
       <c r="X69" s="41"/>
@@ -5962,19 +5976,19 @@
       <c r="N70" s="31">
         <v>5.555555555555555</v>
       </c>
-      <c r="O70" s="34"/>
-      <c r="P70" s="34"/>
+      <c r="O70" s="38"/>
+      <c r="P70" s="38"/>
       <c r="Q70" s="30"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="37">
+      <c r="R70" s="38"/>
+      <c r="S70" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T70" s="38">
+      <c r="T70" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U70" s="34"/>
+      <c r="U70" s="38"/>
       <c r="V70" s="41"/>
       <c r="W70" s="41"/>
       <c r="X70" s="41"/>
@@ -6009,19 +6023,19 @@
       <c r="N71" s="31">
         <v>3.888888888888889</v>
       </c>
-      <c r="O71" s="34"/>
-      <c r="P71" s="34"/>
+      <c r="O71" s="38"/>
+      <c r="P71" s="38"/>
       <c r="Q71" s="30"/>
-      <c r="R71" s="34"/>
-      <c r="S71" s="37">
+      <c r="R71" s="38"/>
+      <c r="S71" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T71" s="38">
+      <c r="T71" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U71" s="34"/>
+      <c r="U71" s="38"/>
       <c r="V71" s="41"/>
       <c r="W71" s="41"/>
       <c r="X71" s="41"/>
@@ -6068,21 +6082,21 @@
       <c r="N72" s="31">
         <v>1.305</v>
       </c>
-      <c r="O72" s="34">
+      <c r="O72" s="38">
         <v>1.0</v>
       </c>
-      <c r="P72" s="34"/>
+      <c r="P72" s="38"/>
       <c r="Q72" s="30"/>
-      <c r="R72" s="34"/>
-      <c r="S72" s="37">
+      <c r="R72" s="38"/>
+      <c r="S72" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T72" s="38">
+      <c r="T72" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U72" s="34" t="s">
+      <c r="U72" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V72" s="41"/>
@@ -6119,19 +6133,19 @@
       <c r="N73" s="31">
         <v>1.6433333333333333</v>
       </c>
-      <c r="O73" s="34"/>
-      <c r="P73" s="34"/>
+      <c r="O73" s="38"/>
+      <c r="P73" s="38"/>
       <c r="Q73" s="30"/>
-      <c r="R73" s="34"/>
-      <c r="S73" s="37">
+      <c r="R73" s="38"/>
+      <c r="S73" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T73" s="38">
+      <c r="T73" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U73" s="34"/>
+      <c r="U73" s="38"/>
       <c r="V73" s="41"/>
       <c r="W73" s="41"/>
       <c r="X73" s="41"/>
@@ -6166,19 +6180,19 @@
       <c r="N74" s="31">
         <v>1.765</v>
       </c>
-      <c r="O74" s="34"/>
-      <c r="P74" s="34"/>
+      <c r="O74" s="38"/>
+      <c r="P74" s="38"/>
       <c r="Q74" s="30"/>
-      <c r="R74" s="34"/>
-      <c r="S74" s="37">
+      <c r="R74" s="38"/>
+      <c r="S74" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T74" s="38">
+      <c r="T74" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U74" s="34"/>
+      <c r="U74" s="38"/>
       <c r="V74" s="41"/>
       <c r="W74" s="41"/>
       <c r="X74" s="41"/>
@@ -6213,19 +6227,19 @@
       <c r="N75" s="31">
         <v>1.445</v>
       </c>
-      <c r="O75" s="34"/>
-      <c r="P75" s="34"/>
+      <c r="O75" s="38"/>
+      <c r="P75" s="38"/>
       <c r="Q75" s="30"/>
-      <c r="R75" s="34"/>
-      <c r="S75" s="37">
+      <c r="R75" s="38"/>
+      <c r="S75" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T75" s="38">
+      <c r="T75" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U75" s="34"/>
+      <c r="U75" s="38"/>
       <c r="V75" s="41"/>
       <c r="W75" s="41"/>
       <c r="X75" s="41"/>
@@ -6272,21 +6286,21 @@
       <c r="N76" s="31">
         <v>5.555555555555555</v>
       </c>
-      <c r="O76" s="34"/>
-      <c r="P76" s="34">
+      <c r="O76" s="38"/>
+      <c r="P76" s="38">
         <v>2.0</v>
       </c>
       <c r="Q76" s="30"/>
-      <c r="R76" s="34"/>
-      <c r="S76" s="37">
+      <c r="R76" s="38"/>
+      <c r="S76" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T76" s="38">
+      <c r="T76" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U76" s="34"/>
+      <c r="U76" s="38"/>
       <c r="V76" s="41"/>
       <c r="W76" s="41"/>
       <c r="X76" s="41"/>
@@ -6321,19 +6335,19 @@
       <c r="N77" s="31">
         <v>6.111111111111111</v>
       </c>
-      <c r="O77" s="34"/>
-      <c r="P77" s="34"/>
+      <c r="O77" s="38"/>
+      <c r="P77" s="38"/>
       <c r="Q77" s="30"/>
-      <c r="R77" s="34"/>
-      <c r="S77" s="37">
+      <c r="R77" s="38"/>
+      <c r="S77" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T77" s="38">
+      <c r="T77" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U77" s="34"/>
+      <c r="U77" s="38"/>
       <c r="V77" s="41"/>
       <c r="W77" s="41"/>
       <c r="X77" s="41"/>
@@ -6380,21 +6394,21 @@
       <c r="N78" s="31">
         <v>2.296666666666667</v>
       </c>
-      <c r="O78" s="34"/>
-      <c r="P78" s="34">
+      <c r="O78" s="38"/>
+      <c r="P78" s="38">
         <v>2.0</v>
       </c>
       <c r="Q78" s="30"/>
-      <c r="R78" s="34"/>
-      <c r="S78" s="37">
+      <c r="R78" s="38"/>
+      <c r="S78" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T78" s="38">
+      <c r="T78" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U78" s="34"/>
+      <c r="U78" s="38"/>
       <c r="V78" s="41"/>
       <c r="W78" s="41"/>
       <c r="X78" s="41"/>
@@ -6429,19 +6443,19 @@
       <c r="N79" s="31">
         <v>3.5620000000000003</v>
       </c>
-      <c r="O79" s="34"/>
-      <c r="P79" s="34"/>
+      <c r="O79" s="38"/>
+      <c r="P79" s="38"/>
       <c r="Q79" s="30"/>
-      <c r="R79" s="34"/>
-      <c r="S79" s="37">
+      <c r="R79" s="38"/>
+      <c r="S79" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T79" s="38">
+      <c r="T79" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U79" s="34"/>
+      <c r="U79" s="38"/>
       <c r="V79" s="41"/>
       <c r="W79" s="41"/>
       <c r="X79" s="41"/>
@@ -6476,19 +6490,19 @@
       <c r="N80" s="31">
         <v>3.8176666666666668</v>
       </c>
-      <c r="O80" s="34"/>
-      <c r="P80" s="34"/>
+      <c r="O80" s="38"/>
+      <c r="P80" s="38"/>
       <c r="Q80" s="30"/>
-      <c r="R80" s="34"/>
-      <c r="S80" s="37">
+      <c r="R80" s="38"/>
+      <c r="S80" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T80" s="38">
+      <c r="T80" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U80" s="34"/>
+      <c r="U80" s="38"/>
       <c r="V80" s="41"/>
       <c r="W80" s="41"/>
       <c r="X80" s="41"/>
@@ -6523,19 +6537,19 @@
       <c r="N81" s="31">
         <v>3.8523333333333336</v>
       </c>
-      <c r="O81" s="34"/>
-      <c r="P81" s="34"/>
+      <c r="O81" s="38"/>
+      <c r="P81" s="38"/>
       <c r="Q81" s="30"/>
-      <c r="R81" s="34"/>
-      <c r="S81" s="37">
+      <c r="R81" s="38"/>
+      <c r="S81" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T81" s="38">
+      <c r="T81" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U81" s="34"/>
+      <c r="U81" s="38"/>
       <c r="V81" s="41"/>
       <c r="W81" s="41"/>
       <c r="X81" s="41"/>
@@ -6582,21 +6596,21 @@
       <c r="N82" s="31">
         <v>3.0</v>
       </c>
-      <c r="O82" s="34"/>
-      <c r="P82" s="34">
+      <c r="O82" s="38"/>
+      <c r="P82" s="38">
         <v>2.0</v>
       </c>
       <c r="Q82" s="30"/>
-      <c r="R82" s="34"/>
-      <c r="S82" s="37">
+      <c r="R82" s="38"/>
+      <c r="S82" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T82" s="38">
+      <c r="T82" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U82" s="34"/>
+      <c r="U82" s="38"/>
       <c r="V82" s="41"/>
       <c r="W82" s="41"/>
       <c r="X82" s="41"/>
@@ -6631,19 +6645,19 @@
       <c r="N83" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O83" s="34"/>
-      <c r="P83" s="34"/>
+      <c r="O83" s="38"/>
+      <c r="P83" s="38"/>
       <c r="Q83" s="30"/>
-      <c r="R83" s="34"/>
-      <c r="S83" s="37">
+      <c r="R83" s="38"/>
+      <c r="S83" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T83" s="38">
+      <c r="T83" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U83" s="34"/>
+      <c r="U83" s="38"/>
       <c r="V83" s="41"/>
       <c r="W83" s="41"/>
       <c r="X83" s="41"/>
@@ -6678,19 +6692,19 @@
       <c r="N84" s="31">
         <v>2.6666666666666665</v>
       </c>
-      <c r="O84" s="34"/>
-      <c r="P84" s="34"/>
+      <c r="O84" s="38"/>
+      <c r="P84" s="38"/>
       <c r="Q84" s="30"/>
-      <c r="R84" s="34"/>
-      <c r="S84" s="37">
+      <c r="R84" s="38"/>
+      <c r="S84" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T84" s="38">
+      <c r="T84" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U84" s="34"/>
+      <c r="U84" s="38"/>
       <c r="V84" s="41"/>
       <c r="W84" s="41"/>
       <c r="X84" s="41"/>
@@ -6725,19 +6739,19 @@
       <c r="N85" s="31">
         <v>2.3333333333333335</v>
       </c>
-      <c r="O85" s="34"/>
-      <c r="P85" s="34"/>
+      <c r="O85" s="38"/>
+      <c r="P85" s="38"/>
       <c r="Q85" s="30"/>
-      <c r="R85" s="34"/>
-      <c r="S85" s="37">
+      <c r="R85" s="38"/>
+      <c r="S85" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T85" s="38">
+      <c r="T85" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U85" s="34"/>
+      <c r="U85" s="38"/>
       <c r="V85" s="41"/>
       <c r="W85" s="41"/>
       <c r="X85" s="41"/>
@@ -6784,21 +6798,21 @@
       <c r="N86" s="31">
         <v>3.0</v>
       </c>
-      <c r="O86" s="34"/>
-      <c r="P86" s="34">
+      <c r="O86" s="38"/>
+      <c r="P86" s="38">
         <v>2.0</v>
       </c>
       <c r="Q86" s="30"/>
-      <c r="R86" s="34"/>
-      <c r="S86" s="37">
+      <c r="R86" s="38"/>
+      <c r="S86" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T86" s="38">
+      <c r="T86" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U86" s="34"/>
+      <c r="U86" s="38"/>
       <c r="V86" s="41"/>
       <c r="W86" s="41"/>
       <c r="X86" s="41"/>
@@ -6833,19 +6847,19 @@
       <c r="N87" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O87" s="34"/>
-      <c r="P87" s="34"/>
+      <c r="O87" s="38"/>
+      <c r="P87" s="38"/>
       <c r="Q87" s="30"/>
-      <c r="R87" s="34"/>
-      <c r="S87" s="37">
+      <c r="R87" s="38"/>
+      <c r="S87" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T87" s="38">
+      <c r="T87" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U87" s="34"/>
+      <c r="U87" s="38"/>
       <c r="V87" s="41"/>
       <c r="W87" s="41"/>
       <c r="X87" s="41"/>
@@ -6880,19 +6894,19 @@
       <c r="N88" s="31">
         <v>2.6666666666666665</v>
       </c>
-      <c r="O88" s="34"/>
-      <c r="P88" s="34"/>
+      <c r="O88" s="38"/>
+      <c r="P88" s="38"/>
       <c r="Q88" s="30"/>
-      <c r="R88" s="34"/>
-      <c r="S88" s="37">
+      <c r="R88" s="38"/>
+      <c r="S88" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T88" s="38">
+      <c r="T88" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U88" s="34"/>
+      <c r="U88" s="38"/>
       <c r="V88" s="41"/>
       <c r="W88" s="41"/>
       <c r="X88" s="41"/>
@@ -6927,19 +6941,19 @@
       <c r="N89" s="31">
         <v>3.1866666666666665</v>
       </c>
-      <c r="O89" s="34"/>
-      <c r="P89" s="34"/>
+      <c r="O89" s="38"/>
+      <c r="P89" s="38"/>
       <c r="Q89" s="30"/>
-      <c r="R89" s="34"/>
-      <c r="S89" s="37">
+      <c r="R89" s="38"/>
+      <c r="S89" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T89" s="38">
+      <c r="T89" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U89" s="34"/>
+      <c r="U89" s="38"/>
       <c r="V89" s="41"/>
       <c r="W89" s="41"/>
       <c r="X89" s="41"/>
@@ -6974,19 +6988,19 @@
       <c r="N90" s="31">
         <v>3.1866666666666665</v>
       </c>
-      <c r="O90" s="34"/>
-      <c r="P90" s="34"/>
+      <c r="O90" s="38"/>
+      <c r="P90" s="38"/>
       <c r="Q90" s="30"/>
-      <c r="R90" s="34"/>
-      <c r="S90" s="37">
+      <c r="R90" s="38"/>
+      <c r="S90" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T90" s="38">
+      <c r="T90" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U90" s="34"/>
+      <c r="U90" s="38"/>
       <c r="V90" s="41"/>
       <c r="W90" s="41"/>
       <c r="X90" s="41"/>
@@ -7033,21 +7047,21 @@
       <c r="N91" s="31">
         <v>3.3333333333333335</v>
       </c>
-      <c r="O91" s="34"/>
-      <c r="P91" s="34">
+      <c r="O91" s="38"/>
+      <c r="P91" s="38">
         <v>2.0</v>
       </c>
       <c r="Q91" s="30"/>
-      <c r="R91" s="34"/>
-      <c r="S91" s="37">
+      <c r="R91" s="38"/>
+      <c r="S91" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T91" s="38">
+      <c r="T91" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U91" s="34"/>
+      <c r="U91" s="38"/>
       <c r="V91" s="41"/>
       <c r="W91" s="41"/>
       <c r="X91" s="41"/>
@@ -7082,19 +7096,19 @@
       <c r="N92" s="31">
         <v>3.388888888888889</v>
       </c>
-      <c r="O92" s="34"/>
-      <c r="P92" s="34"/>
+      <c r="O92" s="38"/>
+      <c r="P92" s="38"/>
       <c r="Q92" s="30"/>
-      <c r="R92" s="34"/>
-      <c r="S92" s="37">
+      <c r="R92" s="38"/>
+      <c r="S92" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T92" s="38">
+      <c r="T92" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U92" s="34"/>
+      <c r="U92" s="38"/>
       <c r="V92" s="41"/>
       <c r="W92" s="41"/>
       <c r="X92" s="41"/>
@@ -7129,19 +7143,19 @@
       <c r="N93" s="31">
         <v>3.2222222222222223</v>
       </c>
-      <c r="O93" s="34"/>
-      <c r="P93" s="34"/>
+      <c r="O93" s="38"/>
+      <c r="P93" s="38"/>
       <c r="Q93" s="30"/>
-      <c r="R93" s="34"/>
-      <c r="S93" s="37">
+      <c r="R93" s="38"/>
+      <c r="S93" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T93" s="38">
+      <c r="T93" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U93" s="34"/>
+      <c r="U93" s="38"/>
       <c r="V93" s="41"/>
       <c r="W93" s="41"/>
       <c r="X93" s="41"/>
@@ -7176,19 +7190,19 @@
       <c r="N94" s="31">
         <v>3.8333333333333335</v>
       </c>
-      <c r="O94" s="34"/>
-      <c r="P94" s="34"/>
+      <c r="O94" s="38"/>
+      <c r="P94" s="38"/>
       <c r="Q94" s="30"/>
-      <c r="R94" s="34"/>
-      <c r="S94" s="37">
+      <c r="R94" s="38"/>
+      <c r="S94" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T94" s="38">
+      <c r="T94" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U94" s="34"/>
+      <c r="U94" s="38"/>
       <c r="V94" s="41"/>
       <c r="W94" s="41"/>
       <c r="X94" s="41"/>
@@ -7223,19 +7237,19 @@
       <c r="N95" s="31">
         <v>2.5</v>
       </c>
-      <c r="O95" s="34"/>
-      <c r="P95" s="34"/>
+      <c r="O95" s="38"/>
+      <c r="P95" s="38"/>
       <c r="Q95" s="30"/>
-      <c r="R95" s="34"/>
-      <c r="S95" s="37">
+      <c r="R95" s="38"/>
+      <c r="S95" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T95" s="38">
+      <c r="T95" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U95" s="34"/>
+      <c r="U95" s="38"/>
       <c r="V95" s="41"/>
       <c r="W95" s="41"/>
       <c r="X95" s="41"/>
@@ -7282,21 +7296,21 @@
       <c r="N96" s="31">
         <v>2.5</v>
       </c>
-      <c r="O96" s="34"/>
-      <c r="P96" s="34">
+      <c r="O96" s="38"/>
+      <c r="P96" s="38">
         <v>2.0</v>
       </c>
       <c r="Q96" s="30"/>
-      <c r="R96" s="34"/>
-      <c r="S96" s="37">
+      <c r="R96" s="38"/>
+      <c r="S96" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T96" s="38">
+      <c r="T96" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U96" s="34"/>
+      <c r="U96" s="38"/>
       <c r="V96" s="41"/>
       <c r="W96" s="41"/>
       <c r="X96" s="41"/>
@@ -7343,21 +7357,21 @@
       <c r="N97" s="31">
         <v>4.0</v>
       </c>
-      <c r="O97" s="34"/>
-      <c r="P97" s="34">
+      <c r="O97" s="38"/>
+      <c r="P97" s="38">
         <v>2.0</v>
       </c>
       <c r="Q97" s="30"/>
-      <c r="R97" s="34"/>
-      <c r="S97" s="37">
+      <c r="R97" s="38"/>
+      <c r="S97" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T97" s="38">
+      <c r="T97" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U97" s="34"/>
+      <c r="U97" s="38"/>
       <c r="V97" s="41"/>
       <c r="W97" s="41"/>
       <c r="X97" s="41"/>
@@ -7392,19 +7406,19 @@
       <c r="N98" s="31">
         <v>4.666666666666667</v>
       </c>
-      <c r="O98" s="34"/>
-      <c r="P98" s="34"/>
+      <c r="O98" s="38"/>
+      <c r="P98" s="38"/>
       <c r="Q98" s="30"/>
-      <c r="R98" s="34"/>
-      <c r="S98" s="37">
+      <c r="R98" s="38"/>
+      <c r="S98" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T98" s="38">
+      <c r="T98" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U98" s="34"/>
+      <c r="U98" s="38"/>
       <c r="V98" s="41"/>
       <c r="W98" s="41"/>
       <c r="X98" s="41"/>
@@ -7439,19 +7453,19 @@
       <c r="N99" s="31">
         <v>5.333333333333333</v>
       </c>
-      <c r="O99" s="34"/>
-      <c r="P99" s="34"/>
+      <c r="O99" s="38"/>
+      <c r="P99" s="38"/>
       <c r="Q99" s="30"/>
-      <c r="R99" s="34"/>
-      <c r="S99" s="37">
+      <c r="R99" s="38"/>
+      <c r="S99" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T99" s="38">
+      <c r="T99" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U99" s="34"/>
+      <c r="U99" s="38"/>
       <c r="V99" s="41"/>
       <c r="W99" s="41"/>
       <c r="X99" s="41"/>
@@ -7486,19 +7500,19 @@
       <c r="N100" s="31">
         <v>6.666666666666667</v>
       </c>
-      <c r="O100" s="34"/>
-      <c r="P100" s="34"/>
+      <c r="O100" s="38"/>
+      <c r="P100" s="38"/>
       <c r="Q100" s="30"/>
-      <c r="R100" s="34"/>
-      <c r="S100" s="37">
+      <c r="R100" s="38"/>
+      <c r="S100" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T100" s="38">
+      <c r="T100" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U100" s="34"/>
+      <c r="U100" s="38"/>
       <c r="V100" s="41"/>
       <c r="W100" s="41"/>
       <c r="X100" s="41"/>
@@ -7533,19 +7547,19 @@
       <c r="N101" s="31">
         <v>8.0</v>
       </c>
-      <c r="O101" s="34"/>
-      <c r="P101" s="34"/>
+      <c r="O101" s="38"/>
+      <c r="P101" s="38"/>
       <c r="Q101" s="30"/>
-      <c r="R101" s="34"/>
-      <c r="S101" s="37">
+      <c r="R101" s="38"/>
+      <c r="S101" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T101" s="38">
+      <c r="T101" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U101" s="34"/>
+      <c r="U101" s="38"/>
       <c r="V101" s="41"/>
       <c r="W101" s="41"/>
       <c r="X101" s="41"/>
@@ -7580,19 +7594,19 @@
       <c r="N102" s="31">
         <v>8.0</v>
       </c>
-      <c r="O102" s="34"/>
-      <c r="P102" s="34"/>
+      <c r="O102" s="38"/>
+      <c r="P102" s="38"/>
       <c r="Q102" s="30"/>
-      <c r="R102" s="34"/>
-      <c r="S102" s="37">
+      <c r="R102" s="38"/>
+      <c r="S102" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T102" s="38">
+      <c r="T102" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U102" s="34"/>
+      <c r="U102" s="38"/>
       <c r="V102" s="41"/>
       <c r="W102" s="41"/>
       <c r="X102" s="41"/>
@@ -7639,21 +7653,21 @@
       <c r="N103" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O103" s="34"/>
-      <c r="P103" s="34">
+      <c r="O103" s="38"/>
+      <c r="P103" s="38">
         <v>2.0</v>
       </c>
       <c r="Q103" s="30"/>
-      <c r="R103" s="34"/>
-      <c r="S103" s="37">
+      <c r="R103" s="38"/>
+      <c r="S103" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T103" s="38">
+      <c r="T103" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U103" s="34"/>
+      <c r="U103" s="38"/>
       <c r="V103" s="41"/>
       <c r="W103" s="41"/>
       <c r="X103" s="41"/>
@@ -7688,19 +7702,19 @@
       <c r="N104" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O104" s="34"/>
-      <c r="P104" s="34"/>
+      <c r="O104" s="38"/>
+      <c r="P104" s="38"/>
       <c r="Q104" s="30"/>
-      <c r="R104" s="34"/>
-      <c r="S104" s="37">
+      <c r="R104" s="38"/>
+      <c r="S104" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T104" s="38">
+      <c r="T104" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U104" s="34"/>
+      <c r="U104" s="38"/>
       <c r="V104" s="41"/>
       <c r="W104" s="41"/>
       <c r="X104" s="41"/>
@@ -7735,19 +7749,19 @@
       <c r="N105" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O105" s="34"/>
-      <c r="P105" s="34"/>
+      <c r="O105" s="38"/>
+      <c r="P105" s="38"/>
       <c r="Q105" s="30"/>
-      <c r="R105" s="34"/>
-      <c r="S105" s="37">
+      <c r="R105" s="38"/>
+      <c r="S105" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T105" s="38">
+      <c r="T105" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U105" s="34"/>
+      <c r="U105" s="38"/>
       <c r="V105" s="41"/>
       <c r="W105" s="41"/>
       <c r="X105" s="41"/>
@@ -7782,19 +7796,19 @@
       <c r="N106" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O106" s="34"/>
-      <c r="P106" s="34"/>
+      <c r="O106" s="38"/>
+      <c r="P106" s="38"/>
       <c r="Q106" s="30"/>
-      <c r="R106" s="34"/>
-      <c r="S106" s="37">
+      <c r="R106" s="38"/>
+      <c r="S106" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T106" s="38">
+      <c r="T106" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U106" s="34"/>
+      <c r="U106" s="38"/>
       <c r="V106" s="41"/>
       <c r="W106" s="41"/>
       <c r="X106" s="41"/>
@@ -7829,19 +7843,19 @@
       <c r="N107" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O107" s="34"/>
-      <c r="P107" s="34"/>
+      <c r="O107" s="38"/>
+      <c r="P107" s="38"/>
       <c r="Q107" s="30"/>
-      <c r="R107" s="34"/>
-      <c r="S107" s="37">
+      <c r="R107" s="38"/>
+      <c r="S107" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T107" s="38">
+      <c r="T107" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U107" s="34"/>
+      <c r="U107" s="38"/>
       <c r="V107" s="41"/>
       <c r="W107" s="41"/>
       <c r="X107" s="41"/>
@@ -7876,19 +7890,19 @@
       <c r="N108" s="31">
         <v>13.88888888888889</v>
       </c>
-      <c r="O108" s="34"/>
-      <c r="P108" s="34"/>
+      <c r="O108" s="38"/>
+      <c r="P108" s="38"/>
       <c r="Q108" s="30"/>
-      <c r="R108" s="34"/>
-      <c r="S108" s="37">
+      <c r="R108" s="38"/>
+      <c r="S108" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T108" s="38">
+      <c r="T108" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U108" s="34"/>
+      <c r="U108" s="38"/>
       <c r="V108" s="41"/>
       <c r="W108" s="41"/>
       <c r="X108" s="41"/>
@@ -7935,21 +7949,21 @@
       <c r="N109" s="31">
         <v>2.9166666666666665</v>
       </c>
-      <c r="O109" s="34"/>
-      <c r="P109" s="34">
+      <c r="O109" s="38"/>
+      <c r="P109" s="38">
         <v>2.0</v>
       </c>
       <c r="Q109" s="30"/>
-      <c r="R109" s="34"/>
-      <c r="S109" s="37">
+      <c r="R109" s="38"/>
+      <c r="S109" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T109" s="38">
+      <c r="T109" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U109" s="34"/>
+      <c r="U109" s="38"/>
       <c r="V109" s="41"/>
       <c r="W109" s="41"/>
       <c r="X109" s="41"/>
@@ -7982,19 +7996,19 @@
       <c r="N110" s="31">
         <v>2.9166666666666665</v>
       </c>
-      <c r="O110" s="34"/>
-      <c r="P110" s="34"/>
+      <c r="O110" s="38"/>
+      <c r="P110" s="38"/>
       <c r="Q110" s="30"/>
-      <c r="R110" s="34"/>
-      <c r="S110" s="37">
+      <c r="R110" s="38"/>
+      <c r="S110" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T110" s="38">
+      <c r="T110" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U110" s="34"/>
+      <c r="U110" s="38"/>
       <c r="V110" s="41"/>
       <c r="W110" s="41"/>
       <c r="X110" s="41"/>
@@ -8041,21 +8055,21 @@
       <c r="N111" s="31">
         <v>5.0</v>
       </c>
-      <c r="O111" s="34"/>
-      <c r="P111" s="34">
+      <c r="O111" s="38"/>
+      <c r="P111" s="38">
         <v>2.0</v>
       </c>
       <c r="Q111" s="30"/>
-      <c r="R111" s="34"/>
-      <c r="S111" s="37">
+      <c r="R111" s="38"/>
+      <c r="S111" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T111" s="38">
+      <c r="T111" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U111" s="34"/>
+      <c r="U111" s="38"/>
       <c r="V111" s="41"/>
       <c r="W111" s="41"/>
       <c r="X111" s="41"/>
@@ -8102,21 +8116,21 @@
       <c r="N112" s="31">
         <v>1.9444444444444444</v>
       </c>
-      <c r="O112" s="34"/>
-      <c r="P112" s="34">
+      <c r="O112" s="38"/>
+      <c r="P112" s="38">
         <v>2.0</v>
       </c>
       <c r="Q112" s="30"/>
-      <c r="R112" s="34"/>
-      <c r="S112" s="37">
+      <c r="R112" s="38"/>
+      <c r="S112" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T112" s="38">
+      <c r="T112" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U112" s="34"/>
+      <c r="U112" s="38"/>
       <c r="V112" s="41"/>
       <c r="W112" s="41"/>
       <c r="X112" s="41"/>
@@ -8151,19 +8165,19 @@
       <c r="N113" s="31">
         <v>2.2222222222222223</v>
       </c>
-      <c r="O113" s="34"/>
-      <c r="P113" s="34"/>
+      <c r="O113" s="38"/>
+      <c r="P113" s="38"/>
       <c r="Q113" s="30"/>
-      <c r="R113" s="34"/>
-      <c r="S113" s="37">
+      <c r="R113" s="38"/>
+      <c r="S113" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T113" s="38">
+      <c r="T113" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U113" s="34"/>
+      <c r="U113" s="38"/>
       <c r="V113" s="41"/>
       <c r="W113" s="41"/>
       <c r="X113" s="41"/>
@@ -8198,19 +8212,19 @@
       <c r="N114" s="31">
         <v>2.2222222222222223</v>
       </c>
-      <c r="O114" s="34"/>
-      <c r="P114" s="34"/>
+      <c r="O114" s="38"/>
+      <c r="P114" s="38"/>
       <c r="Q114" s="30"/>
-      <c r="R114" s="34"/>
-      <c r="S114" s="37">
+      <c r="R114" s="38"/>
+      <c r="S114" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T114" s="38">
+      <c r="T114" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U114" s="34"/>
+      <c r="U114" s="38"/>
       <c r="V114" s="41"/>
       <c r="W114" s="41"/>
       <c r="X114" s="41"/>
@@ -8245,19 +8259,19 @@
       <c r="N115" s="31">
         <v>1.9444444444444444</v>
       </c>
-      <c r="O115" s="34"/>
-      <c r="P115" s="34"/>
+      <c r="O115" s="38"/>
+      <c r="P115" s="38"/>
       <c r="Q115" s="30"/>
-      <c r="R115" s="34"/>
-      <c r="S115" s="37">
+      <c r="R115" s="38"/>
+      <c r="S115" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T115" s="38">
+      <c r="T115" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U115" s="34"/>
+      <c r="U115" s="38"/>
       <c r="V115" s="41"/>
       <c r="W115" s="41"/>
       <c r="X115" s="41"/>
@@ -8304,21 +8318,21 @@
       <c r="N116" s="31">
         <v>6.3</v>
       </c>
-      <c r="O116" s="34"/>
-      <c r="P116" s="34">
+      <c r="O116" s="38"/>
+      <c r="P116" s="38">
         <v>2.0</v>
       </c>
       <c r="Q116" s="30"/>
-      <c r="R116" s="34"/>
-      <c r="S116" s="37">
+      <c r="R116" s="38"/>
+      <c r="S116" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T116" s="38">
+      <c r="T116" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U116" s="34"/>
+      <c r="U116" s="38"/>
       <c r="V116" s="41"/>
       <c r="W116" s="41"/>
       <c r="X116" s="41"/>
@@ -8353,19 +8367,19 @@
       <c r="N117" s="31">
         <v>4.5</v>
       </c>
-      <c r="O117" s="34"/>
-      <c r="P117" s="34"/>
+      <c r="O117" s="38"/>
+      <c r="P117" s="38"/>
       <c r="Q117" s="30"/>
-      <c r="R117" s="34"/>
-      <c r="S117" s="37">
+      <c r="R117" s="38"/>
+      <c r="S117" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T117" s="38">
+      <c r="T117" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U117" s="34"/>
+      <c r="U117" s="38"/>
       <c r="V117" s="41"/>
       <c r="W117" s="41"/>
       <c r="X117" s="41"/>
@@ -8400,19 +8414,19 @@
       <c r="N118" s="31">
         <v>5.4</v>
       </c>
-      <c r="O118" s="34"/>
-      <c r="P118" s="34"/>
+      <c r="O118" s="38"/>
+      <c r="P118" s="38"/>
       <c r="Q118" s="30"/>
-      <c r="R118" s="34"/>
-      <c r="S118" s="37">
+      <c r="R118" s="38"/>
+      <c r="S118" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T118" s="38">
+      <c r="T118" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U118" s="34"/>
+      <c r="U118" s="38"/>
       <c r="V118" s="41"/>
       <c r="W118" s="41"/>
       <c r="X118" s="41"/>
@@ -8459,21 +8473,21 @@
       <c r="N119" s="31">
         <v>1.9444444444444444</v>
       </c>
-      <c r="O119" s="34"/>
-      <c r="P119" s="34">
+      <c r="O119" s="38"/>
+      <c r="P119" s="38">
         <v>2.0</v>
       </c>
       <c r="Q119" s="30"/>
-      <c r="R119" s="34"/>
-      <c r="S119" s="37">
+      <c r="R119" s="38"/>
+      <c r="S119" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T119" s="38">
+      <c r="T119" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U119" s="34" t="s">
+      <c r="U119" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V119" s="41"/>
@@ -8510,19 +8524,19 @@
       <c r="N120" s="31">
         <v>2.5</v>
       </c>
-      <c r="O120" s="34"/>
-      <c r="P120" s="34"/>
+      <c r="O120" s="38"/>
+      <c r="P120" s="38"/>
       <c r="Q120" s="30"/>
-      <c r="R120" s="34"/>
-      <c r="S120" s="37">
+      <c r="R120" s="38"/>
+      <c r="S120" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T120" s="38">
+      <c r="T120" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U120" s="34"/>
+      <c r="U120" s="38"/>
       <c r="V120" s="41"/>
       <c r="W120" s="41"/>
       <c r="X120" s="41"/>
@@ -8557,19 +8571,19 @@
       <c r="N121" s="31">
         <v>2.5</v>
       </c>
-      <c r="O121" s="34"/>
-      <c r="P121" s="34"/>
+      <c r="O121" s="38"/>
+      <c r="P121" s="38"/>
       <c r="Q121" s="30"/>
-      <c r="R121" s="34"/>
-      <c r="S121" s="37">
+      <c r="R121" s="38"/>
+      <c r="S121" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T121" s="38">
+      <c r="T121" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U121" s="34"/>
+      <c r="U121" s="38"/>
       <c r="V121" s="41"/>
       <c r="W121" s="41"/>
       <c r="X121" s="41"/>
@@ -8604,19 +8618,19 @@
       <c r="N122" s="31">
         <v>2.7777777777777777</v>
       </c>
-      <c r="O122" s="34"/>
-      <c r="P122" s="34"/>
+      <c r="O122" s="38"/>
+      <c r="P122" s="38"/>
       <c r="Q122" s="30"/>
-      <c r="R122" s="34"/>
-      <c r="S122" s="37">
+      <c r="R122" s="38"/>
+      <c r="S122" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T122" s="38">
+      <c r="T122" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U122" s="34"/>
+      <c r="U122" s="38"/>
       <c r="V122" s="41"/>
       <c r="W122" s="41"/>
       <c r="X122" s="41"/>
@@ -8663,19 +8677,19 @@
       <c r="N123" s="31">
         <v>2.1666666666666665</v>
       </c>
-      <c r="O123" s="34"/>
-      <c r="P123" s="34"/>
+      <c r="O123" s="38"/>
+      <c r="P123" s="38"/>
       <c r="Q123" s="30"/>
-      <c r="R123" s="34"/>
-      <c r="S123" s="37">
+      <c r="R123" s="38"/>
+      <c r="S123" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T123" s="38">
+      <c r="T123" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U123" s="34" t="s">
+      <c r="U123" s="38" t="s">
         <v>98</v>
       </c>
       <c r="V123" s="41"/>
@@ -8714,19 +8728,19 @@
       <c r="N124" s="31">
         <v>2.5277777777777777</v>
       </c>
-      <c r="O124" s="34"/>
-      <c r="P124" s="34"/>
+      <c r="O124" s="38"/>
+      <c r="P124" s="38"/>
       <c r="Q124" s="30"/>
-      <c r="R124" s="34"/>
-      <c r="S124" s="37">
+      <c r="R124" s="38"/>
+      <c r="S124" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T124" s="38">
+      <c r="T124" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U124" s="34"/>
+      <c r="U124" s="38"/>
       <c r="V124" s="41"/>
       <c r="W124" s="41"/>
       <c r="X124" s="41"/>
@@ -8752,13 +8766,13 @@
       <c r="L125" s="30"/>
       <c r="M125" s="31"/>
       <c r="N125" s="31"/>
-      <c r="O125" s="34"/>
-      <c r="P125" s="34"/>
+      <c r="O125" s="38"/>
+      <c r="P125" s="38"/>
       <c r="Q125" s="30"/>
-      <c r="R125" s="34"/>
+      <c r="R125" s="38"/>
       <c r="S125" s="44"/>
       <c r="T125" s="44"/>
-      <c r="U125" s="34"/>
+      <c r="U125" s="38"/>
       <c r="V125" s="41"/>
       <c r="W125" s="41"/>
       <c r="X125" s="41"/>
@@ -8784,13 +8798,13 @@
       <c r="L126" s="30"/>
       <c r="M126" s="31"/>
       <c r="N126" s="31"/>
-      <c r="O126" s="34"/>
-      <c r="P126" s="34"/>
+      <c r="O126" s="38"/>
+      <c r="P126" s="38"/>
       <c r="Q126" s="30"/>
-      <c r="R126" s="34"/>
+      <c r="R126" s="38"/>
       <c r="S126" s="44"/>
       <c r="T126" s="44"/>
-      <c r="U126" s="34"/>
+      <c r="U126" s="38"/>
       <c r="V126" s="41"/>
       <c r="W126" s="41"/>
       <c r="X126" s="41"/>
@@ -8816,13 +8830,13 @@
       <c r="L127" s="30"/>
       <c r="M127" s="31"/>
       <c r="N127" s="31"/>
-      <c r="O127" s="34"/>
-      <c r="P127" s="34"/>
+      <c r="O127" s="38"/>
+      <c r="P127" s="38"/>
       <c r="Q127" s="30"/>
-      <c r="R127" s="34"/>
+      <c r="R127" s="38"/>
       <c r="S127" s="44"/>
       <c r="T127" s="44"/>
-      <c r="U127" s="34"/>
+      <c r="U127" s="38"/>
       <c r="V127" s="41"/>
       <c r="W127" s="41"/>
       <c r="X127" s="41"/>
@@ -8848,13 +8862,13 @@
       <c r="L128" s="30"/>
       <c r="M128" s="31"/>
       <c r="N128" s="31"/>
-      <c r="O128" s="34"/>
-      <c r="P128" s="34"/>
+      <c r="O128" s="38"/>
+      <c r="P128" s="38"/>
       <c r="Q128" s="30"/>
-      <c r="R128" s="34"/>
+      <c r="R128" s="38"/>
       <c r="S128" s="44"/>
       <c r="T128" s="44"/>
-      <c r="U128" s="34"/>
+      <c r="U128" s="38"/>
       <c r="V128" s="41"/>
       <c r="W128" s="41"/>
       <c r="X128" s="41"/>
@@ -8880,13 +8894,13 @@
       <c r="L129" s="30"/>
       <c r="M129" s="31"/>
       <c r="N129" s="31"/>
-      <c r="O129" s="34"/>
-      <c r="P129" s="34"/>
+      <c r="O129" s="38"/>
+      <c r="P129" s="38"/>
       <c r="Q129" s="30"/>
-      <c r="R129" s="34"/>
+      <c r="R129" s="38"/>
       <c r="S129" s="44"/>
       <c r="T129" s="44"/>
-      <c r="U129" s="34"/>
+      <c r="U129" s="38"/>
       <c r="V129" s="41"/>
       <c r="W129" s="41"/>
       <c r="X129" s="41"/>
@@ -8912,13 +8926,13 @@
       <c r="L130" s="30"/>
       <c r="M130" s="31"/>
       <c r="N130" s="31"/>
-      <c r="O130" s="34"/>
-      <c r="P130" s="34"/>
+      <c r="O130" s="38"/>
+      <c r="P130" s="38"/>
       <c r="Q130" s="30"/>
-      <c r="R130" s="34"/>
+      <c r="R130" s="38"/>
       <c r="S130" s="44"/>
       <c r="T130" s="44"/>
-      <c r="U130" s="34"/>
+      <c r="U130" s="38"/>
       <c r="V130" s="41"/>
       <c r="W130" s="41"/>
       <c r="X130" s="41"/>
@@ -8944,13 +8958,13 @@
       <c r="L131" s="30"/>
       <c r="M131" s="31"/>
       <c r="N131" s="31"/>
-      <c r="O131" s="34"/>
-      <c r="P131" s="34"/>
+      <c r="O131" s="38"/>
+      <c r="P131" s="38"/>
       <c r="Q131" s="30"/>
-      <c r="R131" s="34"/>
+      <c r="R131" s="38"/>
       <c r="S131" s="44"/>
       <c r="T131" s="44"/>
-      <c r="U131" s="34"/>
+      <c r="U131" s="38"/>
       <c r="V131" s="41"/>
       <c r="W131" s="41"/>
       <c r="X131" s="41"/>
@@ -8976,13 +8990,13 @@
       <c r="L132" s="30"/>
       <c r="M132" s="31"/>
       <c r="N132" s="31"/>
-      <c r="O132" s="34"/>
-      <c r="P132" s="34"/>
+      <c r="O132" s="38"/>
+      <c r="P132" s="38"/>
       <c r="Q132" s="30"/>
-      <c r="R132" s="34"/>
+      <c r="R132" s="38"/>
       <c r="S132" s="44"/>
       <c r="T132" s="44"/>
-      <c r="U132" s="34"/>
+      <c r="U132" s="38"/>
       <c r="V132" s="41"/>
       <c r="W132" s="41"/>
       <c r="X132" s="41"/>
@@ -9008,13 +9022,13 @@
       <c r="L133" s="30"/>
       <c r="M133" s="31"/>
       <c r="N133" s="31"/>
-      <c r="O133" s="34"/>
-      <c r="P133" s="34"/>
+      <c r="O133" s="38"/>
+      <c r="P133" s="38"/>
       <c r="Q133" s="30"/>
-      <c r="R133" s="34"/>
+      <c r="R133" s="38"/>
       <c r="S133" s="44"/>
       <c r="T133" s="44"/>
-      <c r="U133" s="34"/>
+      <c r="U133" s="38"/>
       <c r="V133" s="41"/>
       <c r="W133" s="41"/>
       <c r="X133" s="41"/>
@@ -9040,13 +9054,13 @@
       <c r="L134" s="30"/>
       <c r="M134" s="31"/>
       <c r="N134" s="31"/>
-      <c r="O134" s="34"/>
-      <c r="P134" s="34"/>
+      <c r="O134" s="38"/>
+      <c r="P134" s="38"/>
       <c r="Q134" s="30"/>
-      <c r="R134" s="34"/>
+      <c r="R134" s="38"/>
       <c r="S134" s="44"/>
       <c r="T134" s="44"/>
-      <c r="U134" s="34"/>
+      <c r="U134" s="38"/>
       <c r="V134" s="41"/>
       <c r="W134" s="41"/>
       <c r="X134" s="41"/>
@@ -9072,13 +9086,13 @@
       <c r="L135" s="30"/>
       <c r="M135" s="31"/>
       <c r="N135" s="31"/>
-      <c r="O135" s="34"/>
-      <c r="P135" s="34"/>
+      <c r="O135" s="38"/>
+      <c r="P135" s="38"/>
       <c r="Q135" s="30"/>
-      <c r="R135" s="34"/>
+      <c r="R135" s="38"/>
       <c r="S135" s="44"/>
       <c r="T135" s="44"/>
-      <c r="U135" s="34"/>
+      <c r="U135" s="38"/>
       <c r="V135" s="41"/>
       <c r="W135" s="41"/>
       <c r="X135" s="41"/>
@@ -9171,19 +9185,19 @@
       <c r="P138" s="68"/>
       <c r="Q138" s="64">
         <f t="shared" ref="Q138:R138" si="4">SUM(Q9:Q137)</f>
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="R138" s="68">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>510</v>
       </c>
       <c r="S138" s="69">
         <f>(Q138+R138)/G138</f>
-        <v>0.0001319330835</v>
+        <v>0.006662620719</v>
       </c>
       <c r="T138" s="67">
         <f>SUM(T9:T137)</f>
-        <v>0.05555555556</v>
+        <v>2.805555556</v>
       </c>
       <c r="U138" s="68"/>
       <c r="V138" s="70"/>

</xml_diff>